<commit_message>
solve the warning message and update the method
</commit_message>
<xml_diff>
--- a/pop_chara_table.xlsx
+++ b/pop_chara_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuhe/Desktop/CU Spring 2023/master thesis II2/CU_2023_yu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF43B7BB-DFF1-F044-82E6-8BE65A0D7C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31083DE1-A7C0-9D4E-8BF0-67F7285BC9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34540" yWindow="-20560" windowWidth="21600" windowHeight="37900" xr2:uid="{0D0941E5-CE22-8240-9DB6-AF088B500D2C}"/>
+    <workbookView xWindow="12900" yWindow="760" windowWidth="21600" windowHeight="20060" activeTab="2" xr2:uid="{0D0941E5-CE22-8240-9DB6-AF088B500D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1352,6 +1352,30 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1373,9 +1397,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1384,27 +1405,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8449D95-32DA-FC41-9F52-AD235BA1BAA6}">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1738,7 +1738,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="57" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1750,15 +1750,15 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="59" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" thickBot="1">
-      <c r="A3" s="50"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="2" t="s">
         <v>133</v>
       </c>
@@ -1768,42 +1768,42 @@
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:8" ht="17">
       <c r="A4" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="55">
-        <v>3797</v>
-      </c>
-      <c r="F4" s="57"/>
+      <c r="E4" s="54">
+        <v>3797</v>
+      </c>
+      <c r="F4" s="64"/>
     </row>
     <row r="5" spans="1:8" ht="17">
       <c r="A5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="58"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="65"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2160,14 +2160,14 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="8">
         <v>3797</v>
       </c>
@@ -2317,14 +2317,14 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="45" customHeight="1">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
       <c r="G29" s="8">
         <v>3797</v>
       </c>
@@ -2535,14 +2535,14 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="8">
         <v>3797</v>
       </c>
@@ -2571,10 +2571,10 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="63" t="s">
+      <c r="A41" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="59"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="10"/>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -2632,10 +2632,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="64" t="s">
+      <c r="A44" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="64"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="17"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -2845,10 +2845,10 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="63" t="s">
+      <c r="A53" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="59"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
@@ -3005,7 +3005,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="34">
-      <c r="A62" s="60" t="s">
+      <c r="A62" s="52" t="s">
         <v>95</v>
       </c>
       <c r="B62" s="21" t="s">
@@ -3017,15 +3017,15 @@
       <c r="D62" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="55" t="s">
+      <c r="E62" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F62" s="55" t="s">
+      <c r="F62" s="54" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18" thickBot="1">
-      <c r="A63" s="61"/>
+      <c r="A63" s="53"/>
       <c r="B63" s="22" t="s">
         <v>1</v>
       </c>
@@ -3035,14 +3035,14 @@
       <c r="D63" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E63" s="62"/>
-      <c r="F63" s="62"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="55"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="64" t="s">
+      <c r="A64" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="64"/>
+      <c r="B64" s="51"/>
       <c r="C64" s="5"/>
       <c r="D64" s="23"/>
       <c r="E64" s="6"/>
@@ -3097,10 +3097,10 @@
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="63" t="s">
+      <c r="A67" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="59"/>
+      <c r="B67" s="50"/>
       <c r="C67" s="24"/>
       <c r="D67" s="25"/>
       <c r="E67" s="25"/>
@@ -3155,10 +3155,10 @@
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="64" t="s">
+      <c r="A70" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="64"/>
+      <c r="B70" s="51"/>
       <c r="C70" s="23"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -3213,10 +3213,10 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="65" t="s">
+      <c r="A73" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="B73" s="65"/>
+      <c r="B73" s="48"/>
       <c r="C73" s="24"/>
       <c r="D73" s="25"/>
       <c r="E73" s="25"/>
@@ -3391,10 +3391,10 @@
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="64" t="s">
+      <c r="A81" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B81" s="64"/>
+      <c r="B81" s="51"/>
       <c r="C81" s="5"/>
       <c r="D81" s="23"/>
       <c r="E81" s="6"/>
@@ -3545,10 +3545,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="17" customHeight="1">
-      <c r="A88" s="65" t="s">
+      <c r="A88" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="B88" s="65"/>
+      <c r="B88" s="48"/>
       <c r="C88" s="24"/>
       <c r="D88" s="25"/>
       <c r="E88" s="25"/>
@@ -3699,10 +3699,10 @@
       </c>
     </row>
     <row r="95" spans="1:7">
-      <c r="A95" s="64" t="s">
+      <c r="A95" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="B95" s="64"/>
+      <c r="B95" s="51"/>
       <c r="C95" s="5"/>
       <c r="D95" s="23"/>
       <c r="E95" s="6"/>
@@ -3853,10 +3853,10 @@
       </c>
     </row>
     <row r="102" spans="1:7">
-      <c r="A102" s="65" t="s">
+      <c r="A102" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="B102" s="65"/>
+      <c r="B102" s="48"/>
       <c r="C102" s="24"/>
       <c r="D102" s="25"/>
       <c r="E102" s="25"/>
@@ -4007,10 +4007,10 @@
       </c>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="64" t="s">
+      <c r="A109" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="B109" s="64"/>
+      <c r="B109" s="51"/>
       <c r="C109" s="5"/>
       <c r="D109" s="23"/>
       <c r="E109" s="6"/>
@@ -4161,10 +4161,10 @@
       </c>
     </row>
     <row r="116" spans="1:7">
-      <c r="A116" s="63" t="s">
+      <c r="A116" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B116" s="59"/>
+      <c r="B116" s="50"/>
       <c r="C116" s="24"/>
       <c r="D116" s="25"/>
       <c r="E116" s="25"/>
@@ -4219,10 +4219,10 @@
       </c>
     </row>
     <row r="119" spans="1:7">
-      <c r="A119" s="64" t="s">
+      <c r="A119" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="B119" s="64"/>
+      <c r="B119" s="51"/>
       <c r="C119" s="5"/>
       <c r="D119" s="23"/>
       <c r="E119" s="6"/>
@@ -4301,10 +4301,10 @@
       </c>
     </row>
     <row r="123" spans="1:7">
-      <c r="A123" s="63" t="s">
+      <c r="A123" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="B123" s="59"/>
+      <c r="B123" s="50"/>
       <c r="C123" s="24"/>
       <c r="D123" s="25"/>
       <c r="E123" s="25"/>
@@ -4383,10 +4383,10 @@
       </c>
     </row>
     <row r="127" spans="1:7">
-      <c r="A127" s="64" t="s">
+      <c r="A127" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="B127" s="64"/>
+      <c r="B127" s="51"/>
       <c r="C127" s="5"/>
       <c r="D127" s="23"/>
       <c r="E127" s="6"/>
@@ -4465,10 +4465,10 @@
       </c>
     </row>
     <row r="131" spans="1:7">
-      <c r="A131" s="65" t="s">
+      <c r="A131" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="B131" s="65"/>
+      <c r="B131" s="48"/>
       <c r="C131" s="24"/>
       <c r="D131" s="25"/>
       <c r="E131" s="25"/>
@@ -4644,6 +4644,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="A131:B131"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A123:B123"/>
@@ -4660,22 +4676,6 @@
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A29:F29"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4699,8 +4699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E47EFE70-F573-7549-A8CF-94CEDB3059A0}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4715,7 +4715,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="34">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="59" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4727,15 +4727,15 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="59" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickBot="1">
-      <c r="A3" s="52"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -4745,42 +4745,42 @@
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:7" ht="17">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="61">
         <v>713</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="61">
         <v>1843</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="61">
         <v>167</v>
       </c>
-      <c r="E4" s="55">
-        <v>2723</v>
-      </c>
-      <c r="F4" s="57"/>
+      <c r="E4" s="54">
+        <v>2723</v>
+      </c>
+      <c r="F4" s="64"/>
     </row>
     <row r="5" spans="1:7" ht="17">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="58"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="65"/>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -5147,14 +5147,14 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
       <c r="G22" s="8">
         <v>2723</v>
       </c>
@@ -5208,14 +5208,14 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
       <c r="G25" s="8">
         <v>2723</v>
       </c>
@@ -5341,14 +5341,14 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="8">
         <v>2723</v>
       </c>
@@ -5556,14 +5556,14 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="48" t="s">
+      <c r="A41" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
     </row>
     <row r="42" spans="1:7" ht="51" customHeight="1">
       <c r="A42" s="8" t="s">
@@ -5586,10 +5586,10 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="63" t="s">
+      <c r="A43" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="59"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="10"/>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -5644,10 +5644,10 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="17"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -5846,10 +5846,10 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="63" t="s">
+      <c r="A55" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="59"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
@@ -6008,7 +6008,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="34">
-      <c r="A64" s="55" t="s">
+      <c r="A64" s="54" t="s">
         <v>95</v>
       </c>
       <c r="B64" s="21" t="s">
@@ -6020,15 +6020,15 @@
       <c r="D64" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="55" t="s">
+      <c r="E64" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F64" s="55" t="s">
+      <c r="F64" s="54" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18" thickBot="1">
-      <c r="A65" s="62"/>
+      <c r="A65" s="55"/>
       <c r="B65" s="22" t="s">
         <v>1</v>
       </c>
@@ -6038,14 +6038,14 @@
       <c r="D65" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E65" s="62"/>
-      <c r="F65" s="62"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="55"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="64" t="s">
+      <c r="A66" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="64"/>
+      <c r="B66" s="51"/>
       <c r="C66" s="5"/>
       <c r="D66" s="23"/>
       <c r="E66" s="6"/>
@@ -6100,10 +6100,10 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="63" t="s">
+      <c r="A69" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B69" s="59"/>
+      <c r="B69" s="50"/>
       <c r="C69" s="24"/>
       <c r="D69" s="25"/>
       <c r="E69" s="25"/>
@@ -6161,10 +6161,10 @@
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="64" t="s">
+      <c r="A72" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="64"/>
+      <c r="B72" s="51"/>
       <c r="C72" s="23"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
@@ -6222,10 +6222,10 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="65" t="s">
+      <c r="A75" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="B75" s="65"/>
+      <c r="B75" s="48"/>
       <c r="C75" s="24"/>
       <c r="D75" s="25"/>
       <c r="E75" s="25"/>
@@ -6403,10 +6403,10 @@
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="64" t="s">
+      <c r="A83" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B83" s="64"/>
+      <c r="B83" s="51"/>
       <c r="C83" s="5"/>
       <c r="D83" s="23"/>
       <c r="E83" s="6"/>
@@ -6560,10 +6560,10 @@
       </c>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="65" t="s">
+      <c r="A90" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="B90" s="65"/>
+      <c r="B90" s="48"/>
       <c r="C90" s="24"/>
       <c r="D90" s="25"/>
       <c r="E90" s="25"/>
@@ -6717,10 +6717,10 @@
       </c>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="64" t="s">
+      <c r="A97" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="B97" s="64"/>
+      <c r="B97" s="51"/>
       <c r="C97" s="5"/>
       <c r="D97" s="23"/>
       <c r="E97" s="6"/>
@@ -6874,10 +6874,10 @@
       </c>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="65" t="s">
+      <c r="A104" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="B104" s="65"/>
+      <c r="B104" s="48"/>
       <c r="C104" s="24"/>
       <c r="D104" s="25"/>
       <c r="E104" s="25"/>
@@ -7031,10 +7031,10 @@
       </c>
     </row>
     <row r="111" spans="1:7">
-      <c r="A111" s="64" t="s">
+      <c r="A111" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="B111" s="64"/>
+      <c r="B111" s="51"/>
       <c r="C111" s="5"/>
       <c r="D111" s="23"/>
       <c r="E111" s="6"/>
@@ -7188,10 +7188,10 @@
       </c>
     </row>
     <row r="118" spans="1:7">
-      <c r="A118" s="63" t="s">
+      <c r="A118" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B118" s="59"/>
+      <c r="B118" s="50"/>
       <c r="C118" s="24"/>
       <c r="D118" s="25"/>
       <c r="E118" s="25"/>
@@ -7249,10 +7249,10 @@
       </c>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="64" t="s">
+      <c r="A121" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="B121" s="64"/>
+      <c r="B121" s="51"/>
       <c r="C121" s="5"/>
       <c r="D121" s="23"/>
       <c r="E121" s="6"/>
@@ -7334,10 +7334,10 @@
       </c>
     </row>
     <row r="125" spans="1:7">
-      <c r="A125" s="63" t="s">
+      <c r="A125" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="B125" s="59"/>
+      <c r="B125" s="50"/>
       <c r="C125" s="24"/>
       <c r="D125" s="25"/>
       <c r="E125" s="25"/>
@@ -7419,10 +7419,10 @@
       </c>
     </row>
     <row r="129" spans="1:7">
-      <c r="A129" s="64" t="s">
+      <c r="A129" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="B129" s="64"/>
+      <c r="B129" s="51"/>
       <c r="C129" s="5"/>
       <c r="D129" s="23"/>
       <c r="E129" s="6"/>
@@ -7504,10 +7504,10 @@
       </c>
     </row>
     <row r="133" spans="1:7">
-      <c r="A133" s="65" t="s">
+      <c r="A133" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="B133" s="65"/>
+      <c r="B133" s="48"/>
       <c r="C133" s="24"/>
       <c r="D133" s="25"/>
       <c r="E133" s="25"/>
@@ -7686,15 +7686,14 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="A133:B133"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A75:B75"/>
@@ -7711,14 +7710,15 @@
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A55:B55"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>